<commit_message>
Repository for Connections and Main Configuration
</commit_message>
<xml_diff>
--- a/InputOutputFiles/IEC_104_Conf.xlsx
+++ b/InputOutputFiles/IEC_104_Conf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Useful\Priv\Programming\_VS_Projects\WAGO_CodesysV23_Protocols\InputOutputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30E4967-65D2-41C4-A253-819C149636FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F3F710-6A71-4729-A0F7-F8D83B04C7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{852913BC-0740-468B-9F45-217D065EB444}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{852913BC-0740-468B-9F45-217D065EB444}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Configuration" sheetId="3" r:id="rId1"/>
@@ -167,15 +167,6 @@
     <t>Client104-001_ClientConnection104-001</t>
   </si>
   <si>
-    <t>ExecutionTimeDefault</t>
-  </si>
-  <si>
-    <t>ExecutionTimeShort</t>
-  </si>
-  <si>
-    <t>ExecutionTimeLong</t>
-  </si>
-  <si>
     <t>t#2s</t>
   </si>
   <si>
@@ -183,6 +174,15 @@
   </si>
   <si>
     <t>t#5s</t>
+  </si>
+  <si>
+    <t>Execution Time Default</t>
+  </si>
+  <si>
+    <t>Execution Time Short</t>
+  </si>
+  <si>
+    <t>Execution Time Long</t>
   </si>
 </sst>
 </file>
@@ -560,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C83666C1-86BF-4346-82B6-7EACDD2157DE}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,24 +573,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -603,7 +603,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,7 +706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72D27F81-CBAF-4521-81D0-D05BDC6A7D6F}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added WagoTime handling in Excel.DataAccess
</commit_message>
<xml_diff>
--- a/InputOutputFiles/IEC_104_Conf.xlsx
+++ b/InputOutputFiles/IEC_104_Conf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Useful\Priv\Programming\_VS_Projects\WAGO_CodesysV23_Protocols\InputOutputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F3F710-6A71-4729-A0F7-F8D83B04C7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D9624E-5A21-4D74-AABE-D78FF9741570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{852913BC-0740-468B-9F45-217D065EB444}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{852913BC-0740-468B-9F45-217D065EB444}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Configuration" sheetId="3" r:id="rId1"/>
@@ -560,7 +560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C83666C1-86BF-4346-82B6-7EACDD2157DE}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -706,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72D27F81-CBAF-4521-81D0-D05BDC6A7D6F}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>